<commit_message>
Parses csv files and sends corresponding texts
</commit_message>
<xml_diff>
--- a/PASTE_Demo_Info.xlsx
+++ b/PASTE_Demo_Info.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="186" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{CC5652D4-7F91-4E75-8A24-B318AAAD2F42}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew\Documents\astartups\EMAApp-node\EMA-Texting-Application\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C62B542-DACA-472B-87F7-37600DA9E2DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="58">
   <si>
     <t>Subject ID #</t>
   </si>
@@ -38,9 +42,6 @@
   </si>
   <si>
     <t>Typical Wake Time</t>
-  </si>
-  <si>
-    <t>Time of Texts &amp; Survey to be sent with text</t>
   </si>
   <si>
     <t>Typical Bed Time</t>
@@ -207,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,14 +241,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -256,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,8 +274,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -634,6 +639,84 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -653,11 +736,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -671,108 +839,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1091,264 +1174,269 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
     <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="15" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
-      <c r="A2" s="12"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="32" t="s">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="29"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="16"/>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="6" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>36</v>
+      <c r="G5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="L5" s="3" t="s">
+    <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="F7" s="32" t="s">
         <v>47</v>
       </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="35"/>
     </row>
-    <row r="7" spans="1:12" ht="21">
-      <c r="F7" s="25" t="s">
+    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="28"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="36"/>
+      <c r="K8" s="37"/>
     </row>
-    <row r="8" spans="1:12" ht="18.75">
-      <c r="F8" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="20" t="s">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="F9" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="38"/>
+      <c r="K9" s="39"/>
     </row>
-    <row r="9" spans="1:12" ht="30">
-      <c r="F9" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="47" t="s">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="48"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
     </row>
-    <row r="10" spans="1:12" ht="45">
-      <c r="F10" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="36" t="s">
+    <row r="11" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="36"/>
-      <c r="K10" s="37"/>
-    </row>
-    <row r="11" spans="1:12" ht="39.75" customHeight="1">
-      <c r="F11" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="16">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I9:K9"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{6B0A1F64-F415-4F8F-8DFF-76E3660CD284}"/>
@@ -1358,5 +1446,6 @@
     <hyperlink ref="I9:K9" r:id="rId5" display="https://goo.gl/forms/EqrRv2KAUDq9ykXo1" xr:uid="{30E6AEAE-C859-448F-A5B6-66CA22FCBDC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>